<commit_message>
.csv file extensions changed to .txt
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\File\GitHub\Married-Couple-Identification\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33368FE-0075-4495-9247-557C7E92DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F3D26-558B-4481-BB5E-5B32B91C0452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3516" yWindow="3516" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="150" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -995,36 +995,24 @@
     <t>customer_id</t>
   </si>
   <si>
-    <t>havale_bil.csv</t>
-  </si>
-  <si>
     <t>transfer</t>
   </si>
   <si>
     <t>customer_age</t>
   </si>
   <si>
-    <t>kk_ekstre_bil.csv</t>
-  </si>
-  <si>
     <t>statement</t>
   </si>
   <si>
     <t>customer_gender</t>
   </si>
   <si>
-    <t>kk_ekstre_odm_bil.csv</t>
-  </si>
-  <si>
     <t>transaction_statement</t>
   </si>
   <si>
     <t>customer_marital_status</t>
   </si>
   <si>
-    <t>kk_har_bilgi.csv</t>
-  </si>
-  <si>
     <t>transaction</t>
   </si>
   <si>
@@ -1035,9 +1023,6 @@
   </si>
   <si>
     <t>customer_education_level</t>
-  </si>
-  <si>
-    <t>sube_isl_ziy.csv</t>
   </si>
   <si>
     <t>branch_visit</t>
@@ -1303,13 +1288,28 @@
     <t>customer_segment</t>
   </si>
   <si>
-    <t>kitle_orneklem_100k.csv</t>
-  </si>
-  <si>
-    <t>atm_islem_xy.csv</t>
-  </si>
-  <si>
     <t>atm</t>
+  </si>
+  <si>
+    <t>havale_bil.txt</t>
+  </si>
+  <si>
+    <t>kk_ekstre_bil.txt</t>
+  </si>
+  <si>
+    <t>kk_ekstre_odm_bil.txt</t>
+  </si>
+  <si>
+    <t>kk_har_bilgi.txt</t>
+  </si>
+  <si>
+    <t>kitle_orneklem_100k.txt</t>
+  </si>
+  <si>
+    <t>sube_isl_ziy.txt</t>
+  </si>
+  <si>
+    <t>atm_islem_xy.txt</t>
   </si>
 </sst>
 </file>
@@ -30991,6 +30991,11 @@
   </sheetData>
   <autoFilter ref="B1:D218" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="A81:A89"/>
+    <mergeCell ref="A90:A97"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="A101:A116"/>
+    <mergeCell ref="A117:A218"/>
     <mergeCell ref="A59:A71"/>
     <mergeCell ref="A72:A80"/>
     <mergeCell ref="G1:I1"/>
@@ -30998,11 +31003,6 @@
     <mergeCell ref="G2:I4"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="A41:A58"/>
-    <mergeCell ref="A81:A89"/>
-    <mergeCell ref="A90:A97"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="A101:A116"/>
-    <mergeCell ref="A117:A218"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -31016,7 +31016,9 @@
   </sheetPr>
   <dimension ref="A1:I218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31079,10 +31081,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>308</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>309</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>53</v>
@@ -31100,16 +31102,16 @@
         <v>11</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" s="5">
         <v>2</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>311</v>
+        <v>397</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>44</v>
@@ -31127,16 +31129,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>314</v>
+        <v>398</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>41</v>
@@ -31154,16 +31156,16 @@
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F5" s="5">
         <v>4</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>317</v>
+        <v>399</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>38</v>
@@ -31181,7 +31183,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F6" s="5">
         <v>5</v>
@@ -31190,7 +31192,7 @@
         <v>400</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>7</v>
@@ -31208,16 +31210,16 @@
         <v>22</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F7" s="5">
         <v>6</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>322</v>
+        <v>401</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>26</v>
@@ -31235,16 +31237,16 @@
         <v>24</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F8" s="20">
         <v>7</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>47</v>
@@ -31274,10 +31276,10 @@
         <v>25</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -31292,7 +31294,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -31307,7 +31309,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -31322,7 +31324,7 @@
         <v>37</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -31341,7 +31343,7 @@
         <v>40</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -31360,7 +31362,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -31379,7 +31381,7 @@
         <v>46</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -31398,7 +31400,7 @@
         <v>49</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -31414,10 +31416,10 @@
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -31455,7 +31457,7 @@
         <v>56</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -31474,7 +31476,7 @@
         <v>59</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -31493,7 +31495,7 @@
         <v>62</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -31512,7 +31514,7 @@
         <v>65</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -31531,7 +31533,7 @@
         <v>68</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -31550,7 +31552,7 @@
         <v>71</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -31588,7 +31590,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -31607,7 +31609,7 @@
         <v>75</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -31626,7 +31628,7 @@
         <v>77</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -31645,7 +31647,7 @@
         <v>79</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -31664,7 +31666,7 @@
         <v>80</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -31683,7 +31685,7 @@
         <v>82</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -31702,7 +31704,7 @@
         <v>84</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -31721,7 +31723,7 @@
         <v>86</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -31740,7 +31742,7 @@
         <v>88</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -31759,7 +31761,7 @@
         <v>90</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -31778,7 +31780,7 @@
         <v>92</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -31871,7 +31873,7 @@
         <v>98</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -31890,7 +31892,7 @@
         <v>100</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -31909,7 +31911,7 @@
         <v>102</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -31947,7 +31949,7 @@
         <v>103</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -31966,7 +31968,7 @@
         <v>105</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -31985,7 +31987,7 @@
         <v>107</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -32004,7 +32006,7 @@
         <v>109</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -32014,7 +32016,7 @@
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24"/>
       <c r="B50" s="19" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>38</v>
@@ -32023,7 +32025,7 @@
         <v>111</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -32042,7 +32044,7 @@
         <v>113</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -32061,7 +32063,7 @@
         <v>115</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -32080,7 +32082,7 @@
         <v>117</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -32099,7 +32101,7 @@
         <v>118</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -32118,7 +32120,7 @@
         <v>119</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -32156,7 +32158,7 @@
         <v>121</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -32175,7 +32177,7 @@
         <v>122</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -32196,7 +32198,7 @@
         <v>125</v>
       </c>
       <c r="E59" s="17" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -32215,7 +32217,7 @@
         <v>126</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -32253,7 +32255,7 @@
         <v>127</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -32272,7 +32274,7 @@
         <v>121</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -32291,7 +32293,7 @@
         <v>129</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -32310,7 +32312,7 @@
         <v>131</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -32329,7 +32331,7 @@
         <v>133</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -32348,7 +32350,7 @@
         <v>135</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -32367,7 +32369,7 @@
         <v>137</v>
       </c>
       <c r="E68" s="17" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -32405,7 +32407,7 @@
         <v>138</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -32424,7 +32426,7 @@
         <v>140</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -32445,7 +32447,7 @@
         <v>143</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -32464,7 +32466,7 @@
         <v>145</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -32483,7 +32485,7 @@
         <v>146</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -32502,7 +32504,7 @@
         <v>148</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -32521,7 +32523,7 @@
         <v>150</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -32556,10 +32558,10 @@
         <v>50</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -32578,7 +32580,7 @@
         <v>153</v>
       </c>
       <c r="E79" s="17" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -32597,7 +32599,7 @@
         <v>155</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -32618,7 +32620,7 @@
         <v>158</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -32637,7 +32639,7 @@
         <v>159</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -32675,7 +32677,7 @@
         <v>160</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -32694,7 +32696,7 @@
         <v>162</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -32713,7 +32715,7 @@
         <v>146</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -32732,7 +32734,7 @@
         <v>163</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -32742,7 +32744,7 @@
     <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="24"/>
       <c r="B88" s="19" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>53</v>
@@ -32751,7 +32753,7 @@
         <v>165</v>
       </c>
       <c r="E88" s="17" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -32770,7 +32772,7 @@
         <v>167</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -32791,7 +32793,7 @@
         <v>93</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -32829,7 +32831,7 @@
         <v>170</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -32848,7 +32850,7 @@
         <v>146</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -32867,7 +32869,7 @@
         <v>172</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -32886,7 +32888,7 @@
         <v>174</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -32905,7 +32907,7 @@
         <v>107</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -32924,7 +32926,7 @@
         <v>177</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -32945,7 +32947,7 @@
         <v>180</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -32983,7 +32985,7 @@
         <v>182</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>

</xml_diff>